<commit_message>
update data add column balance
</commit_message>
<xml_diff>
--- a/data_test_without_type.xlsx
+++ b/data_test_without_type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\volantis\v-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\volantis\v-data\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB6BEE5-8860-40CF-A18A-0C9DFF47D7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728805B-2556-4653-A3B3-5277671F2BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{148D773F-6384-46AB-9FED-C79E430025DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>mikel@essien.com</t>
+  </si>
+  <si>
+    <t>balance</t>
   </si>
 </sst>
 </file>
@@ -432,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31105D62-190F-4261-98E5-0A270483235F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +456,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>121</v>
       </c>
@@ -467,8 +473,11 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1234.3399999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>122</v>
       </c>
@@ -481,8 +490,11 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>1212.23</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>123</v>
       </c>
@@ -492,8 +504,11 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E4">
+        <v>4343.0200000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>124</v>
       </c>
@@ -505,6 +520,9 @@
       </c>
       <c r="D5" t="b">
         <v>1</v>
+      </c>
+      <c r="E5">
+        <v>344.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data add column created_at
</commit_message>
<xml_diff>
--- a/data_test_without_type.xlsx
+++ b/data_test_without_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\volantis\v-data\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728805B-2556-4653-A3B3-5277671F2BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53329FEF-50A7-4B2D-A5ED-35A844159CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{148D773F-6384-46AB-9FED-C79E430025DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>balance</t>
+  </si>
+  <si>
+    <t>created_at</t>
   </si>
 </sst>
 </file>
@@ -117,9 +120,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31105D62-190F-4261-98E5-0A270483235F}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,8 +463,11 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>121</v>
       </c>
@@ -476,8 +483,11 @@
       <c r="E2">
         <v>1234.3399999999999</v>
       </c>
+      <c r="F2" s="2">
+        <v>45325</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>122</v>
       </c>
@@ -493,8 +503,11 @@
       <c r="E3">
         <v>1212.23</v>
       </c>
+      <c r="F3" s="2">
+        <v>45326</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>123</v>
       </c>
@@ -507,8 +520,11 @@
       <c r="E4">
         <v>4343.0200000000004</v>
       </c>
+      <c r="F4" s="2">
+        <v>45327</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>124</v>
       </c>
@@ -523,6 +539,9 @@
       </c>
       <c r="E5">
         <v>344.94</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data add column updated_at
</commit_message>
<xml_diff>
--- a/data_test_without_type.xlsx
+++ b/data_test_without_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\volantis\v-data\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53329FEF-50A7-4B2D-A5ED-35A844159CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A92E32A-44D8-4552-908B-093766AC273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{148D773F-6384-46AB-9FED-C79E430025DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
   </si>
 </sst>
 </file>
@@ -120,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,15 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31105D62-190F-4261-98E5-0A270483235F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="7" max="7" width="14.265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +473,11 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>121</v>
       </c>
@@ -486,8 +496,12 @@
       <c r="F2" s="2">
         <v>45325</v>
       </c>
+      <c r="G2" s="3">
+        <f ca="1">NOW()</f>
+        <v>45406.489142824073</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>122</v>
       </c>
@@ -506,8 +520,12 @@
       <c r="F3" s="2">
         <v>45326</v>
       </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" ca="1" si="0">NOW()</f>
+        <v>45406.489142824073</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>123</v>
       </c>
@@ -523,8 +541,12 @@
       <c r="F4" s="2">
         <v>45327</v>
       </c>
+      <c r="G4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45406.489142824073</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>124</v>
       </c>
@@ -542,6 +564,10 @@
       </c>
       <c r="F5" s="2">
         <v>45328</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>45406.489142824073</v>
       </c>
     </row>
   </sheetData>
@@ -552,5 +578,6 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{3B62D15C-C869-42D5-AD65-AAD424925FE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>